<commit_message>
added more details to architecture
</commit_message>
<xml_diff>
--- a/fox_diffusion/Architectures.xlsx
+++ b/fox_diffusion/Architectures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\dev\Research\fox_diffusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C911FC5-074F-4511-9D85-CA2DE7615856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802D07BD-C9A9-4BA1-A468-FE1397E146D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD70819C-EFA1-4346-BA29-99E9B0E56A54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Paper</t>
   </si>
@@ -68,9 +68,6 @@
     <t>https://arxiv.org/abs/2404.14332</t>
   </si>
   <si>
-    <t>https://arxiv.org/abs/1911.09107</t>
-  </si>
-  <si>
     <t>https://arxiv.org/pdf/2404.18807</t>
   </si>
   <si>
@@ -86,24 +83,72 @@
     <t>Heutsch et al</t>
   </si>
   <si>
-    <t>Dataset set is composed of (t, m) pairs where t is pushed through detector 
+    <t>Results/Limitations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tested for Proton-Proton Collision
+- one simulator for detect/true and other for correction
+- measured performance against six jet substructures
+- from graphs =&gt; distribution pretty closely matched true distribution</t>
+  </si>
+  <si>
+    <t>Results
+- unconditioned encoders performed best
+- VLD models performed best
+- latent models were generally better</t>
+  </si>
+  <si>
+    <t>Problem Statement</t>
+  </si>
+  <si>
+    <t>Solve three challenges regarding current unfolding methods
+- requires observables to be binned into histograms
+- unfold small number of observables
+- all auxiliary features not taken into account</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1911.09107
+https://github.com/hep-lbdl/OmniFold/blob/main/GaussianExample_minimal.ipynb</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dataset set is composed of (t, m) pairs where t is pushed through detector 
 simulation to obtain detector level m
 t have initial weights v_0(t) and when t is pushed to get m, v_0(t) becomes v_0^push(m)
 1. w_n(m) = v_(n - 1)^push(m)L(m)
 - take the weights from the conversion of t to m and multiply with the likelihood ratio from the ML model with the detector level as input
 - w_n^pull(t) = w_n(m) is created by pulling back the w_n to the particle-level weights
-- 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- 3 hidden layers each with 50 nodes and ReLU activation
+- output as Dense layer with sigmoid activation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
 2. v_n(t) = v_n-1(t)L(t)
 - validates the weighting function of the particle-level quantities</t>
-  </si>
-  <si>
-    <t>Results/Limitations</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tested for Proton-Proton Collision
-- one simulator for detect/true and other for correction
-- measured performance against six jet substructures
-- from graphs =&gt; distribution pretty closely matched true distribution</t>
+    </r>
+  </si>
+  <si>
+    <t>Solve current problems regarding SOTA techniques
+- non-ML unfolding methods cannot handle higher dimensions
+- current generative models do not always guarantee samples that respect important physical constraints
+Therefore, diffusion models are used for full-event unfolding where full high-dimensional detector-level observations are mapped to truth-level objects</t>
   </si>
   <si>
     <t>Combines conditioning encoder, data VAE, and diffusion process into single loss function
@@ -115,14 +160,35 @@
 - both conditional and unconditional VAE
 - explore conditioned encoder to estimate VAE posterior but employ uncoditional decoder during generation
 VLD ELBO
-- Refer to (8) in paper for combined ELBO loss</t>
+- Refer to (8) in paper for combined ELBO loss
+Feed-Forward Block
+- ConvNeXt architecture which uses inverted bottleneck
+- inverted bottleneck has 3 linear layers (GELU activation), layer normalization, and gated residual connection
+Detector Encoder
+- follows SPANet architecture
+- uses gated transformer architecture from SPANet v2
+- event-level representations from central transformer encoder
+Parton Encoder
+- starts with embedding layer (fixed 55 dimensional parton -&gt; D-dimensional vector via linear layer)
+- N_e feed-forward blocks arranged in series
+- two independent networks which accept identical input and share same block structure predict mean and log standard deviation
+- normalizing and scaling for mean applied
+Parton Decoder
+- single stack of N_d feed-forward blocks
+- linear D to 55 dimension mapping
+- (conditional) also append D-dimensional detector vector to input
+Denoising Network
+- N_epsilon feed-fowrad blocks
+- maps D-dimensional latent sample z_t to approximate noise that produced it
+- time encoded with 32-dimensional sinusoidal position
+- latent vector, position encoding, and conditioning are concatenated and fed through feed-foward network for noise estimates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,19 +218,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,9 +250,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -532,21 +592,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41309BD6-67A8-45BF-84B8-D1951D26D6A0}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="85.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="5" max="5" width="73.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,89 +619,106 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="267.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2023</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="378" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
         <v>2024</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="267.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2024</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{4C9875EE-A30D-4B01-88A7-5838452ECBDD}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{D0C62E4F-6938-4ED3-BC0E-1C2441B6F98D}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{A8E99C74-1D89-48F8-9031-217A9E79EAB5}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{65EB18B4-46B3-4B01-856A-F48C817F7E63}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{4C9875EE-A30D-4B01-88A7-5838452ECBDD}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{D0C62E4F-6938-4ED3-BC0E-1C2441B6F98D}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{A8E99C74-1D89-48F8-9031-217A9E79EAB5}"/>
+    <hyperlink ref="G4" r:id="rId4" display="https://arxiv.org/abs/1911.09107" xr:uid="{65EB18B4-46B3-4B01-856A-F48C817F7E63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed architecture for Irvine 1.0/2.0
</commit_message>
<xml_diff>
--- a/fox_diffusion/Architectures.xlsx
+++ b/fox_diffusion/Architectures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\dev\Research\fox_diffusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802D07BD-C9A9-4BA1-A468-FE1397E146D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1365378-AE03-4FC2-BDF1-7F67B8CB6E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD70819C-EFA1-4346-BA29-99E9B0E56A54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Paper</t>
   </si>
@@ -151,12 +151,23 @@
 Therefore, diffusion models are used for full-event unfolding where full high-dimensional detector-level observations are mapped to truth-level objects</t>
   </si>
   <si>
-    <t>Combines conditioning encoder, data VAE, and diffusion process into single loss function
+    <r>
+      <t xml:space="preserve">Combines conditioning encoder, data VAE, and diffusion process into single loss function
 Uses a conditional data encoder or decoder
 Conditioning Encoder
 - encoder trained on one objective and then acts as conditioning encoder for another generative model
 - deterministic mapping
-Conditional Parton VAE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Conditional Parton VAE
 - both conditional and unconditional VAE
 - explore conditioned encoder to estimate VAE posterior but employ uncoditional decoder during generation
 VLD ELBO
@@ -168,6 +179,16 @@
 - follows SPANet architecture
 - uses gated transformer architecture from SPANet v2
 - event-level representations from central transformer encoder
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
 Parton Encoder
 - starts with embedding layer (fixed 55 dimensional parton -&gt; D-dimensional vector via linear layer)
 - N_e feed-forward blocks arranged in series
@@ -182,6 +203,37 @@
 - maps D-dimensional latent sample z_t to approximate noise that produced it
 - time encoded with 32-dimensional sinusoidal position
 - latent vector, position encoding, and conditioning are concatenated and fed through feed-foward network for noise estimates</t>
+    </r>
+  </si>
+  <si>
+    <t>OmniFold and VLD work well except they do not account for variable dimensions
+- extension to VLD was introduced to work with variable dimensional set of observables</t>
+  </si>
+  <si>
+    <t>Particle VAE (encoder and decoder)
+- transformer for both encoder and decoder
+- deep feed-forward MLPs applied per-object to reconstruct inputs (fig 5)
+- input includes N particle-level objects complemented by one-hot encoded vector
+Detector Encoder
+- uses identical architecture to particle VAE
+- inputs are M detector-level objcts described with a vector of observables with one-hot encoding of object type
+Multiplicity Predictor
+- encoded detector features is appended with new learnable vectors and is processed with a transformer to extract multiplicity features
+- MLP used to estimate shape and scale parameters of gamma distribution (fig. 7)
+Latent Diffusion Process
+- used diffusion model for conditional distribution
+- diffusion architecture remains same as 2023 paper
+Particle Denoising Network
+- uses a transformer for denoising network
+- particle level inputs are incorporated with fourier positional features and flag vector
+- same approach used for conditioning set
+- noise prediction extracted via dropping transformer outputs for detector-level inputs and indexing the outputs by particle position
+Noise Schedule Network
+- noise schedule parameterized as monotonicaly decreasing function w.r.t time conditiond on position
+- weights are positive
+- inputs: time as scalar and position encoded 
+- one hidden layer with 1000 dimensions with sigmoid activation
+- output is scalar</t>
   </si>
 </sst>
 </file>
@@ -594,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41309BD6-67A8-45BF-84B8-D1951D26D6A0}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -664,14 +716,18 @@
       <c r="C3" s="2">
         <v>2024</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="378" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="252" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
completed architecture excel sheet
</commit_message>
<xml_diff>
--- a/fox_diffusion/Architectures.xlsx
+++ b/fox_diffusion/Architectures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\dev\Research\fox_diffusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1365378-AE03-4FC2-BDF1-7F67B8CB6E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77F1E9-4A33-4A71-BD63-110D4AD66E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD70819C-EFA1-4346-BA29-99E9B0E56A54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Paper</t>
   </si>
@@ -235,12 +235,69 @@
 - one hidden layer with 1000 dimensions with sigmoid activation
 - output is scalar</t>
   </si>
+  <si>
+    <t xml:space="preserve">Layout and extend the ML methods for unfolding
+- tested performance of different models
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Direct Diffusion (he purpose is to find velocity field that transforms density to fit Eq. 18)
+- follows the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Flow matching for generative modeling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> framework from Lipman et al
+- after generative model, ODE with velocity field (encoded in a neural network) 
+    - uses a simple regression task with MSE loss to get the correct velocity field
+- after training =&gt; reconstruction level event is transferred numerically using corresponding ODE in Eq. 16
+- Unpaired Approach (no pairing information)
+    - drop pairing information by modifying conditional trajectory (Eq. 24)
+    - loss function in (Eq. 25)
+- have also tried with Bayesian layers, Gaussian distribution of all/some network parameters, and KL-term regularization
+Latent Diffusion
+- same architecture as Irvine 1.0</t>
+    </r>
+  </si>
+  <si>
+    <t>Results with VLD (Standard Model)
+- excellent agreement in jst multiplicity distribution
+- slight disagreement in low H_T (perhaps due to limited training data?)
+(BSM Injection)
+- with BSM Physics Injection =&gt; slight disagreements similar to standard model results for top quark and tt systems otherwise, good agreement everywhere</t>
+  </si>
+  <si>
+    <t>Detector Unfolding z+ jets
+DiDi
+- worked well with "per-cent precision over entire phase space"
+- worked even better in well-sampled bulk
+- unpaired is slightly less stable
+Latent Diffusion
+- has slightly larger deviation from target distribution
+Unfolding to Parton level
+- VLD did not perform as well compared to conditional flow matching approach</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +333,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -309,6 +373,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -646,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41309BD6-67A8-45BF-84B8-D1951D26D6A0}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +787,9 @@
       <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
@@ -750,7 +817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="252" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -760,10 +827,16 @@
       <c r="C5" s="2">
         <v>2024</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>